<commit_message>
Stan przed sprawdzianem 8.11
</commit_message>
<xml_diff>
--- a/Klasa 4/Excel/Trojkat Pascala - ZD/trojkat.xlsx
+++ b/Klasa 4/Excel/Trojkat Pascala - ZD/trojkat.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Informatyka\Klasa 4\Excel\Trójkąt Pascala - ZD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Informatyka\Klasa 4\Excel\Trojkat Pascala - ZD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{739ABE7E-05F5-42B4-9630-9458EF77351D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{F7EA7DFF-40E7-496A-B7C0-6E6D834DDDBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="normalny" sheetId="1" r:id="rId1"/>
@@ -84,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,21 +457,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E065EE-859F-4B43-8CA1-23A320EBCE37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2">
         <f>A1</f>
         <v>1</v>
@@ -610,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34">
       <c r="A3">
         <f t="shared" ref="A3:A30" si="11">A2</f>
         <v>1</v>
@@ -748,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -886,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34">
       <c r="A5">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1024,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34">
       <c r="A6">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1162,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1300,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1438,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1576,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1714,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1852,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -1990,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2128,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34">
       <c r="A14">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2266,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2404,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="A16">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2542,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34">
       <c r="A17">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2680,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34">
       <c r="A18">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2818,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34">
       <c r="A19">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -2956,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34">
       <c r="A20">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3094,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34">
       <c r="A21">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3232,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34">
       <c r="A22">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3370,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34">
       <c r="A23">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3508,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34">
       <c r="A24">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3646,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34">
       <c r="A25">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3784,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34">
       <c r="A26">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -3922,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34">
       <c r="A27">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -4060,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34">
       <c r="A28">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -4198,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34">
       <c r="A29">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -4336,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34">
       <c r="A30">
         <f t="shared" si="11"/>
         <v>1</v>
@@ -4474,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -4483,7 +4482,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>92378</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35" t="s">
         <v>2</v>
       </c>
@@ -4507,7 +4506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E941F593-D3B6-4B16-B102-33429D81A19D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG65"/>
   <sheetViews>
@@ -4515,12 +4514,12 @@
       <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="AF1" t="s">
         <v>9</v>
       </c>
@@ -4528,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2">
         <f>IF(AND(MOD(normalny!A1,5)=0,normalny!A1&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -4650,14 +4649,14 @@
         <v>0</v>
       </c>
       <c r="AF2">
-        <f>SUM(A2:AD2)</f>
+        <f t="shared" ref="AF2:AF31" si="0">SUM(A2:AD2)</f>
         <v>0</v>
       </c>
       <c r="AG2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3">
         <f>IF(AND(MOD(normalny!A2,5)=0,normalny!A2&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -4779,14 +4778,14 @@
         <v>0</v>
       </c>
       <c r="AF3">
-        <f>SUM(A3:AD3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4">
         <f>IF(AND(MOD(normalny!A3,5)=0,normalny!A3&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -4908,14 +4907,14 @@
         <v>0</v>
       </c>
       <c r="AF4">
-        <f>SUM(A4:AD4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5">
         <f>IF(AND(MOD(normalny!A4,5)=0,normalny!A4&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5037,14 +5036,14 @@
         <v>0</v>
       </c>
       <c r="AF5">
-        <f>SUM(A5:AD5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6">
         <f>IF(AND(MOD(normalny!A5,5)=0,normalny!A5&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5166,14 +5165,14 @@
         <v>0</v>
       </c>
       <c r="AF6">
-        <f>SUM(A6:AD6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7">
         <f>IF(AND(MOD(normalny!A6,5)=0,normalny!A6&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5295,14 +5294,14 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <f>SUM(A7:AD7)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AG7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8">
         <f>IF(AND(MOD(normalny!A7,5)=0,normalny!A7&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5424,14 +5423,14 @@
         <v>0</v>
       </c>
       <c r="AF8">
-        <f>SUM(A8:AD8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AG8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9">
         <f>IF(AND(MOD(normalny!A8,5)=0,normalny!A8&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5553,14 +5552,14 @@
         <v>0</v>
       </c>
       <c r="AF9">
-        <f>SUM(A9:AD9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AG9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10">
         <f>IF(AND(MOD(normalny!A9,5)=0,normalny!A9&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5682,14 +5681,14 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <f>SUM(A10:AD10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AG10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11">
         <f>IF(AND(MOD(normalny!A10,5)=0,normalny!A10&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5811,14 +5810,14 @@
         <v>0</v>
       </c>
       <c r="AF11">
-        <f>SUM(A11:AD11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12">
         <f>IF(AND(MOD(normalny!A11,5)=0,normalny!A11&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -5940,14 +5939,14 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <f>SUM(A12:AD12)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AG12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13">
         <f>IF(AND(MOD(normalny!A12,5)=0,normalny!A12&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6069,14 +6068,14 @@
         <v>0</v>
       </c>
       <c r="AF13">
-        <f>SUM(A13:AD13)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AG13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14">
         <f>IF(AND(MOD(normalny!A13,5)=0,normalny!A13&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6198,14 +6197,14 @@
         <v>0</v>
       </c>
       <c r="AF14">
-        <f>SUM(A14:AD14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AG14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15">
         <f>IF(AND(MOD(normalny!A14,5)=0,normalny!A14&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6327,14 +6326,14 @@
         <v>0</v>
       </c>
       <c r="AF15">
-        <f>SUM(A15:AD15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AG15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33">
       <c r="A16">
         <f>IF(AND(MOD(normalny!A15,5)=0,normalny!A15&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6456,14 +6455,14 @@
         <v>0</v>
       </c>
       <c r="AF16">
-        <f>SUM(A16:AD16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33">
       <c r="A17">
         <f>IF(AND(MOD(normalny!A16,5)=0,normalny!A16&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6585,14 +6584,14 @@
         <v>0</v>
       </c>
       <c r="AF17">
-        <f>SUM(A17:AD17)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="AG17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33">
       <c r="A18">
         <f>IF(AND(MOD(normalny!A17,5)=0,normalny!A17&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6714,14 +6713,14 @@
         <v>0</v>
       </c>
       <c r="AF18">
-        <f>SUM(A18:AD18)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="AG18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33">
       <c r="A19">
         <f>IF(AND(MOD(normalny!A18,5)=0,normalny!A18&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6843,14 +6842,14 @@
         <v>0</v>
       </c>
       <c r="AF19">
-        <f>SUM(A19:AD19)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AG19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33">
       <c r="A20">
         <f>IF(AND(MOD(normalny!A19,5)=0,normalny!A19&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -6972,14 +6971,14 @@
         <v>0</v>
       </c>
       <c r="AF20">
-        <f>SUM(A20:AD20)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AG20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33">
       <c r="A21">
         <f>IF(AND(MOD(normalny!A20,5)=0,normalny!A20&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7101,14 +7100,14 @@
         <v>0</v>
       </c>
       <c r="AF21">
-        <f>SUM(A21:AD21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33">
       <c r="A22">
         <f>IF(AND(MOD(normalny!A21,5)=0,normalny!A21&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7230,14 +7229,14 @@
         <v>0</v>
       </c>
       <c r="AF22">
-        <f>SUM(A22:AD22)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="AG22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33">
       <c r="A23">
         <f>IF(AND(MOD(normalny!A22,5)=0,normalny!A22&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7359,14 +7358,14 @@
         <v>0</v>
       </c>
       <c r="AF23">
-        <f>SUM(A23:AD23)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="AG23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33">
       <c r="A24">
         <f>IF(AND(MOD(normalny!A23,5)=0,normalny!A23&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7488,14 +7487,14 @@
         <v>0</v>
       </c>
       <c r="AF24">
-        <f>SUM(A24:AD24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AG24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33">
       <c r="A25">
         <f>IF(AND(MOD(normalny!A24,5)=0,normalny!A24&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7617,14 +7616,14 @@
         <v>0</v>
       </c>
       <c r="AF25">
-        <f>SUM(A25:AD25)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AG25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33">
       <c r="A26">
         <f>IF(AND(MOD(normalny!A25,5)=0,normalny!A25&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7746,14 +7745,14 @@
         <v>0</v>
       </c>
       <c r="AF26">
-        <f>SUM(A26:AD26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33">
       <c r="A27">
         <f>IF(AND(MOD(normalny!A26,5)=0,normalny!A26&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -7875,14 +7874,14 @@
         <v>0</v>
       </c>
       <c r="AF27">
-        <f>SUM(A27:AD27)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="AG27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33">
       <c r="A28">
         <f>IF(AND(MOD(normalny!A27,5)=0,normalny!A27&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -8004,14 +8003,14 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <f>SUM(A28:AD28)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="AG28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33">
       <c r="A29">
         <f>IF(AND(MOD(normalny!A28,5)=0,normalny!A28&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -8133,14 +8132,14 @@
         <v>0</v>
       </c>
       <c r="AF29">
-        <f>SUM(A29:AD29)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="AG29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33">
       <c r="A30">
         <f>IF(AND(MOD(normalny!A29,5)=0,normalny!A29&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -8262,14 +8261,14 @@
         <v>0</v>
       </c>
       <c r="AF30">
-        <f>SUM(A30:AD30)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="AG30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33">
       <c r="A31">
         <f>IF(AND(MOD(normalny!A30,5)=0,normalny!A30&lt;&gt;0),1,0)</f>
         <v>0</v>
@@ -8391,14 +8390,14 @@
         <v>0</v>
       </c>
       <c r="AF31">
-        <f>SUM(A31:AD31)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="AG31">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="13:14">
       <c r="M35" t="s">
         <v>9</v>
       </c>
@@ -8406,7 +8405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="13:14">
       <c r="M36">
         <v>0</v>
       </c>
@@ -8414,7 +8413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:14">
       <c r="M37">
         <v>0</v>
       </c>
@@ -8422,7 +8421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="13:14">
       <c r="M38">
         <v>0</v>
       </c>
@@ -8430,7 +8429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="13:14">
       <c r="M39">
         <v>0</v>
       </c>
@@ -8438,7 +8437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="13:14">
       <c r="M40">
         <v>0</v>
       </c>
@@ -8446,7 +8445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="13:14" hidden="1">
       <c r="M41">
         <v>4</v>
       </c>
@@ -8454,7 +8453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="13:14" hidden="1">
       <c r="M42">
         <v>3</v>
       </c>
@@ -8462,7 +8461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="13:14" hidden="1">
       <c r="M43">
         <v>2</v>
       </c>
@@ -8470,7 +8469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:14" hidden="1">
       <c r="M44">
         <v>1</v>
       </c>
@@ -8478,7 +8477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="13:14">
       <c r="M45">
         <v>0</v>
       </c>
@@ -8486,7 +8485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="13:14" hidden="1">
       <c r="M46">
         <v>8</v>
       </c>
@@ -8494,7 +8493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:14" hidden="1">
       <c r="M47">
         <v>6</v>
       </c>
@@ -8502,7 +8501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="13:14" hidden="1">
       <c r="M48">
         <v>4</v>
       </c>
@@ -8510,7 +8509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:14" hidden="1">
       <c r="M49">
         <v>2</v>
       </c>
@@ -8518,7 +8517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:14">
       <c r="M50">
         <v>0</v>
       </c>
@@ -8526,7 +8525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:14" hidden="1">
       <c r="M51">
         <v>12</v>
       </c>
@@ -8534,7 +8533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:14" hidden="1">
       <c r="M52">
         <v>9</v>
       </c>
@@ -8542,7 +8541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:14" hidden="1">
       <c r="M53">
         <v>6</v>
       </c>
@@ -8550,7 +8549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:14" hidden="1">
       <c r="M54">
         <v>3</v>
       </c>
@@ -8558,7 +8557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:14">
       <c r="M55">
         <v>0</v>
       </c>
@@ -8566,7 +8565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:14" hidden="1">
       <c r="M56">
         <v>16</v>
       </c>
@@ -8574,7 +8573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:14" hidden="1">
       <c r="M57">
         <v>12</v>
       </c>
@@ -8582,7 +8581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:14" hidden="1">
       <c r="M58">
         <v>8</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:14" hidden="1">
       <c r="M59">
         <v>4</v>
       </c>
@@ -8598,7 +8597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:14">
       <c r="M60">
         <v>0</v>
       </c>
@@ -8606,7 +8605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:14" hidden="1">
       <c r="M61">
         <v>24</v>
       </c>
@@ -8614,7 +8613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:14" hidden="1">
       <c r="M62">
         <v>23</v>
       </c>
@@ -8622,7 +8621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:14" hidden="1">
       <c r="M63">
         <v>22</v>
       </c>
@@ -8630,7 +8629,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:14" hidden="1">
       <c r="M64">
         <v>21</v>
       </c>
@@ -8638,7 +8637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="13:14" hidden="1">
       <c r="M65">
         <v>20</v>
       </c>
@@ -8647,7 +8646,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="M35:N65" xr:uid="{E941F593-D3B6-4B16-B102-33429D81A19D}">
+  <autoFilter ref="M35:N65">
     <filterColumn colId="0">
       <filters>
         <filter val="0"/>
@@ -8659,21 +8658,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F687F805-A6AD-4811-97BB-150739763276}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2:AE31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="AE1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="A2">
         <f>IF(OR(normalny!A1=0, normalny!A1=1),normalny!A1,_xlfn.CEILING.MATH(LOG10(normalny!A1+1),1))</f>
         <v>1</v>
@@ -8799,7 +8798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="A3">
         <f>IF(OR(normalny!A2=0, normalny!A2=1),normalny!A2,_xlfn.CEILING.MATH(LOG10(normalny!A2+1),1))</f>
         <v>1</v>
@@ -8925,7 +8924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="A4">
         <f>IF(OR(normalny!A3=0, normalny!A3=1),normalny!A3,_xlfn.CEILING.MATH(LOG10(normalny!A3+1),1))</f>
         <v>1</v>
@@ -9051,7 +9050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5">
         <f>IF(OR(normalny!A4=0, normalny!A4=1),normalny!A4,_xlfn.CEILING.MATH(LOG10(normalny!A4+1),1))</f>
         <v>1</v>
@@ -9177,7 +9176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6">
         <f>IF(OR(normalny!A5=0, normalny!A5=1),normalny!A5,_xlfn.CEILING.MATH(LOG10(normalny!A5+1),1))</f>
         <v>1</v>
@@ -9303,7 +9302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7">
         <f>IF(OR(normalny!A6=0, normalny!A6=1),normalny!A6,_xlfn.CEILING.MATH(LOG10(normalny!A6+1),1))</f>
         <v>1</v>
@@ -9429,7 +9428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8">
         <f>IF(OR(normalny!A7=0, normalny!A7=1),normalny!A7,_xlfn.CEILING.MATH(LOG10(normalny!A7+1),1))</f>
         <v>1</v>
@@ -9555,7 +9554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9">
         <f>IF(OR(normalny!A8=0, normalny!A8=1),normalny!A8,_xlfn.CEILING.MATH(LOG10(normalny!A8+1),1))</f>
         <v>1</v>
@@ -9681,7 +9680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10">
         <f>IF(OR(normalny!A9=0, normalny!A9=1),normalny!A9,_xlfn.CEILING.MATH(LOG10(normalny!A9+1),1))</f>
         <v>1</v>
@@ -9807,7 +9806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11">
         <f>IF(OR(normalny!A10=0, normalny!A10=1),normalny!A10,_xlfn.CEILING.MATH(LOG10(normalny!A10+1),1))</f>
         <v>1</v>
@@ -9933,7 +9932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12">
         <f>IF(OR(normalny!A11=0, normalny!A11=1),normalny!A11,_xlfn.CEILING.MATH(LOG10(normalny!A11+1),1))</f>
         <v>1</v>
@@ -10059,7 +10058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13">
         <f>IF(OR(normalny!A12=0, normalny!A12=1),normalny!A12,_xlfn.CEILING.MATH(LOG10(normalny!A12+1),1))</f>
         <v>1</v>
@@ -10185,7 +10184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14">
         <f>IF(OR(normalny!A13=0, normalny!A13=1),normalny!A13,_xlfn.CEILING.MATH(LOG10(normalny!A13+1),1))</f>
         <v>1</v>
@@ -10311,7 +10310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15">
         <f>IF(OR(normalny!A14=0, normalny!A14=1),normalny!A14,_xlfn.CEILING.MATH(LOG10(normalny!A14+1),1))</f>
         <v>1</v>
@@ -10437,7 +10436,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16">
         <f>IF(OR(normalny!A15=0, normalny!A15=1),normalny!A15,_xlfn.CEILING.MATH(LOG10(normalny!A15+1),1))</f>
         <v>1</v>
@@ -10563,7 +10562,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17">
         <f>IF(OR(normalny!A16=0, normalny!A16=1),normalny!A16,_xlfn.CEILING.MATH(LOG10(normalny!A16+1),1))</f>
         <v>1</v>
@@ -10689,7 +10688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18">
         <f>IF(OR(normalny!A17=0, normalny!A17=1),normalny!A17,_xlfn.CEILING.MATH(LOG10(normalny!A17+1),1))</f>
         <v>1</v>
@@ -10815,7 +10814,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19">
         <f>IF(OR(normalny!A18=0, normalny!A18=1),normalny!A18,_xlfn.CEILING.MATH(LOG10(normalny!A18+1),1))</f>
         <v>1</v>
@@ -10941,7 +10940,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20">
         <f>IF(OR(normalny!A19=0, normalny!A19=1),normalny!A19,_xlfn.CEILING.MATH(LOG10(normalny!A19+1),1))</f>
         <v>1</v>
@@ -11067,7 +11066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21">
         <f>IF(OR(normalny!A20=0, normalny!A20=1),normalny!A20,_xlfn.CEILING.MATH(LOG10(normalny!A20+1),1))</f>
         <v>1</v>
@@ -11193,7 +11192,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22">
         <f>IF(OR(normalny!A21=0, normalny!A21=1),normalny!A21,_xlfn.CEILING.MATH(LOG10(normalny!A21+1),1))</f>
         <v>1</v>
@@ -11319,7 +11318,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23">
         <f>IF(OR(normalny!A22=0, normalny!A22=1),normalny!A22,_xlfn.CEILING.MATH(LOG10(normalny!A22+1),1))</f>
         <v>1</v>
@@ -11445,7 +11444,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31">
       <c r="A24">
         <f>IF(OR(normalny!A23=0, normalny!A23=1),normalny!A23,_xlfn.CEILING.MATH(LOG10(normalny!A23+1),1))</f>
         <v>1</v>
@@ -11571,7 +11570,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25">
         <f>IF(OR(normalny!A24=0, normalny!A24=1),normalny!A24,_xlfn.CEILING.MATH(LOG10(normalny!A24+1),1))</f>
         <v>1</v>
@@ -11697,7 +11696,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26">
         <f>IF(OR(normalny!A25=0, normalny!A25=1),normalny!A25,_xlfn.CEILING.MATH(LOG10(normalny!A25+1),1))</f>
         <v>1</v>
@@ -11823,7 +11822,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27">
         <f>IF(OR(normalny!A26=0, normalny!A26=1),normalny!A26,_xlfn.CEILING.MATH(LOG10(normalny!A26+1),1))</f>
         <v>1</v>
@@ -11949,7 +11948,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28">
         <f>IF(OR(normalny!A27=0, normalny!A27=1),normalny!A27,_xlfn.CEILING.MATH(LOG10(normalny!A27+1),1))</f>
         <v>1</v>
@@ -12075,7 +12074,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29">
         <f>IF(OR(normalny!A28=0, normalny!A28=1),normalny!A28,_xlfn.CEILING.MATH(LOG10(normalny!A28+1),1))</f>
         <v>1</v>
@@ -12201,7 +12200,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30">
         <f>IF(OR(normalny!A29=0, normalny!A29=1),normalny!A29,_xlfn.CEILING.MATH(LOG10(normalny!A29+1),1))</f>
         <v>1</v>
@@ -12327,7 +12326,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31">
         <f>IF(OR(normalny!A30=0, normalny!A30=1),normalny!A30,_xlfn.CEILING.MATH(LOG10(normalny!A30+1),1))</f>
         <v>1</v>
@@ -12459,30 +12458,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0873E787-167E-49CF-B29E-0EE5CDCAACA3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:6">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:6">
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -12490,7 +12489,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:6">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -12498,7 +12497,7 @@
         <v>92378</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -12506,7 +12505,7 @@
         <v>77558760</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:6">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -12514,7 +12513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -12525,7 +12524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:6">
       <c r="C10">
         <v>1</v>
       </c>
@@ -12536,7 +12535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:6">
       <c r="C11">
         <v>2</v>
       </c>
@@ -12547,7 +12546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:6">
       <c r="C12">
         <v>3</v>
       </c>
@@ -12558,7 +12557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:6">
       <c r="C13">
         <v>4</v>
       </c>
@@ -12569,7 +12568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:6">
       <c r="C14">
         <v>5</v>
       </c>
@@ -12580,7 +12579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:6">
       <c r="C15">
         <v>6</v>
       </c>
@@ -12591,7 +12590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:6">
       <c r="C16">
         <v>7</v>
       </c>
@@ -12602,7 +12601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6">
       <c r="C17">
         <v>8</v>
       </c>
@@ -12613,7 +12612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6">
       <c r="C18">
         <v>9</v>
       </c>
@@ -12624,7 +12623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6">
       <c r="C19">
         <v>10</v>
       </c>
@@ -12632,7 +12631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6">
       <c r="C20">
         <v>11</v>
       </c>
@@ -12640,7 +12639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6">
       <c r="C21">
         <v>12</v>
       </c>
@@ -12648,7 +12647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6">
       <c r="C22">
         <v>13</v>
       </c>
@@ -12656,7 +12655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6">
       <c r="C23">
         <v>14</v>
       </c>
@@ -12664,7 +12663,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6">
       <c r="C24">
         <v>15</v>
       </c>
@@ -12672,7 +12671,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6">
       <c r="C25">
         <v>16</v>
       </c>
@@ -12680,7 +12679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6">
       <c r="C26">
         <v>17</v>
       </c>
@@ -12688,7 +12687,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6">
       <c r="C27">
         <v>18</v>
       </c>
@@ -12696,7 +12695,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6">
       <c r="C28">
         <v>19</v>
       </c>
@@ -12704,7 +12703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6">
       <c r="C29">
         <v>20</v>
       </c>
@@ -12712,7 +12711,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6">
       <c r="C30">
         <v>21</v>
       </c>
@@ -12720,7 +12719,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6">
       <c r="C31">
         <v>22</v>
       </c>
@@ -12728,7 +12727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6">
       <c r="C32">
         <v>23</v>
       </c>
@@ -12736,7 +12735,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4">
       <c r="C33">
         <v>24</v>
       </c>
@@ -12744,7 +12743,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4">
       <c r="C34">
         <v>25</v>
       </c>
@@ -12752,7 +12751,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4">
       <c r="C35">
         <v>26</v>
       </c>
@@ -12760,7 +12759,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4">
       <c r="C36">
         <v>27</v>
       </c>
@@ -12768,7 +12767,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4">
       <c r="C37">
         <v>28</v>
       </c>
@@ -12776,7 +12775,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4">
       <c r="C38">
         <v>29</v>
       </c>
@@ -12784,7 +12783,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4">
       <c r="C39">
         <v>30</v>
       </c>
@@ -12798,19 +12797,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72995D8-55D5-4E37-AEB7-CA86C1327A37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="27" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="str">
         <f>IF(AND(MOD(normalny!A1,3)=0,normalny!A1&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -12932,7 +12931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" t="str">
         <f>IF(AND(MOD(normalny!A2,3)=0,normalny!A2&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13054,7 +13053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" t="str">
         <f>IF(AND(MOD(normalny!A3,3)=0,normalny!A3&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13176,7 +13175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" t="str">
         <f>IF(AND(MOD(normalny!A4,3)=0,normalny!A4&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13298,7 +13297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" t="str">
         <f>IF(AND(MOD(normalny!A5,3)=0,normalny!A5&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13420,7 +13419,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" t="str">
         <f>IF(AND(MOD(normalny!A6,3)=0,normalny!A6&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13542,7 +13541,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" t="str">
         <f>IF(AND(MOD(normalny!A7,3)=0,normalny!A7&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13664,7 +13663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" t="str">
         <f>IF(AND(MOD(normalny!A8,3)=0,normalny!A8&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13786,7 +13785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" t="str">
         <f>IF(AND(MOD(normalny!A9,3)=0,normalny!A9&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -13908,7 +13907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" t="str">
         <f>IF(AND(MOD(normalny!A10,3)=0,normalny!A10&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14030,7 +14029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" t="str">
         <f>IF(AND(MOD(normalny!A11,3)=0,normalny!A11&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14152,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" t="str">
         <f>IF(AND(MOD(normalny!A12,3)=0,normalny!A12&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14274,7 +14273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" t="str">
         <f>IF(AND(MOD(normalny!A13,3)=0,normalny!A13&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14396,7 +14395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" t="str">
         <f>IF(AND(MOD(normalny!A14,3)=0,normalny!A14&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14518,7 +14517,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" t="str">
         <f>IF(AND(MOD(normalny!A15,3)=0,normalny!A15&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14640,7 +14639,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" t="str">
         <f>IF(AND(MOD(normalny!A16,3)=0,normalny!A16&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14762,7 +14761,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17" t="str">
         <f>IF(AND(MOD(normalny!A17,3)=0,normalny!A17&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -14884,7 +14883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18" t="str">
         <f>IF(AND(MOD(normalny!A18,3)=0,normalny!A18&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15006,7 +15005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19" t="str">
         <f>IF(AND(MOD(normalny!A19,3)=0,normalny!A19&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15128,7 +15127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30">
       <c r="A20" t="str">
         <f>IF(AND(MOD(normalny!A20,3)=0,normalny!A20&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15250,7 +15249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" t="str">
         <f>IF(AND(MOD(normalny!A21,3)=0,normalny!A21&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15372,7 +15371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30">
       <c r="A22" t="str">
         <f>IF(AND(MOD(normalny!A22,3)=0,normalny!A22&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15494,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30">
       <c r="A23" t="str">
         <f>IF(AND(MOD(normalny!A23,3)=0,normalny!A23&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15616,7 +15615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24" t="str">
         <f>IF(AND(MOD(normalny!A24,3)=0,normalny!A24&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15738,7 +15737,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25" t="str">
         <f>IF(AND(MOD(normalny!A25,3)=0,normalny!A25&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15860,7 +15859,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26" t="str">
         <f>IF(AND(MOD(normalny!A26,3)=0,normalny!A26&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -15982,7 +15981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30">
       <c r="A27" t="str">
         <f>IF(AND(MOD(normalny!A27,3)=0,normalny!A27&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -16104,7 +16103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30">
       <c r="A28" t="str">
         <f>IF(AND(MOD(normalny!A28,3)=0,normalny!A28&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -16226,7 +16225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30">
       <c r="A29" t="str">
         <f>IF(AND(MOD(normalny!A29,3)=0,normalny!A29&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>
@@ -16348,7 +16347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30">
       <c r="A30" t="str">
         <f>IF(AND(MOD(normalny!A30,3)=0,normalny!A30&lt;&gt;0),"X", " ")</f>
         <v xml:space="preserve"> </v>

</xml_diff>